<commit_message>
Added costing for making 10+ units
Added costing for making 10+ units
</commit_message>
<xml_diff>
--- a/docs/build_instructions_wood_headphonesOnly.xlsx
+++ b/docs/build_instructions_wood_headphonesOnly.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="321" documentId="415E32CF7F9D79DA378485C62B6EEDB6DC1C7F04" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E1E4C037-8CE8-47EA-93BD-87875E7BF0AC}"/>
+  <xr:revisionPtr revIDLastSave="347" documentId="415E32CF7F9D79DA378485C62B6EEDB6DC1C7F04" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1C0F8423-9804-4412-93B9-AA6A987F79C9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_1" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Female-female jumper wires</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Ali Express</t>
   </si>
   <si>
-    <t>M2.5 4mm thread + 6mm standoff screws</t>
-  </si>
-  <si>
     <t># units to make</t>
   </si>
   <si>
@@ -110,6 +107,18 @@
   </si>
   <si>
     <t>16GB micro SD card</t>
+  </si>
+  <si>
+    <t>KY-016 indicator LED (10 pieces)</t>
+  </si>
+  <si>
+    <t>KY-040 rotary encoders (knobs) (5 pieces)</t>
+  </si>
+  <si>
+    <t>M2.5 4mm thread + 6mm standoff screws (30 pieces)</t>
+  </si>
+  <si>
+    <t>+ tax + shipping</t>
   </si>
 </sst>
 </file>
@@ -225,7 +234,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -275,6 +284,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -593,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E12D50-D309-4C94-883F-34F0FBB95462}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,7 +692,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>1</v>
@@ -761,19 +774,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD35BB53-6D32-4D96-AF53-91579E0632D6}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="46.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="35.21875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -782,7 +795,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="12">
         <v>10</v>
@@ -821,13 +834,13 @@
       <c r="F4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>24</v>
+      <c r="G4" s="23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -836,19 +849,19 @@
         <v>10</v>
       </c>
       <c r="D5" s="17">
-        <f>55/24+15</f>
-        <v>17.291666666666668</v>
+        <f>55/10+15+1</f>
+        <v>21.5</v>
       </c>
       <c r="E5" s="17">
         <f t="shared" ref="E5:E15" si="0">C5*D5</f>
-        <v>172.91666666666669</v>
+        <v>215</v>
       </c>
       <c r="F5" s="17">
         <f t="shared" ref="F5:F15" si="1">E5/$B$2</f>
-        <v>17.291666666666668</v>
+        <v>21.5</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -945,7 +958,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>20</v>
@@ -991,7 +1004,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>20</v>
@@ -1014,7 +1027,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>20</v>
@@ -1037,7 +1050,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>1</v>
@@ -1089,9 +1102,11 @@
       <c r="E16" s="12"/>
       <c r="F16" s="21">
         <f>SUM(F5:F15)</f>
-        <v>60.904666666666678</v>
-      </c>
-      <c r="G16" s="12"/>
+        <v>65.113</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1099,12 +1114,12 @@
     <hyperlink ref="A7" r:id="rId2" display="http://www.mcmelectronics.com/product/28-19338" xr:uid="{65D287F0-F3C5-4BFC-B0EB-927314E9D7BC}"/>
     <hyperlink ref="A9" r:id="rId3" xr:uid="{4719F56A-F53F-4C54-AB15-D0404FA4C1F5}"/>
     <hyperlink ref="A8" r:id="rId4" display="http://www.newark.com/mcm/27-5937/3-5mm-inline-stereo-mount-female/dp/40T6284" xr:uid="{EF83C615-A1D4-4987-BEAB-3BBEDC648166}"/>
-    <hyperlink ref="A10" r:id="rId5" xr:uid="{28E7540A-6659-42EF-91A1-7D780614554D}"/>
+    <hyperlink ref="A10" r:id="rId5" display="M2.5 4mm thread + 6mm standoff screws" xr:uid="{28E7540A-6659-42EF-91A1-7D780614554D}"/>
     <hyperlink ref="A14" r:id="rId6" xr:uid="{2A497A6C-5AAE-4A0E-8C0E-F12EF4CC82A4}"/>
     <hyperlink ref="A15" r:id="rId7" display="https://www.amazon.com/SanDisk-16GB-Cruzer-Flash-Drive/dp/B07MDXBT87/ref=sr_1_10?keywords=Cruzer+8GB&amp;qid=1572121525&amp;s=electronics&amp;sr=1-10" xr:uid="{F15FB45E-3203-4F2E-9725-87605B6ECD8B}"/>
     <hyperlink ref="A11" r:id="rId8" xr:uid="{0DC7749B-92C3-4CE4-B5B3-BBC86AC775DE}"/>
-    <hyperlink ref="A12" r:id="rId9" xr:uid="{6A8AA35F-6C88-4BD6-B333-FC1A2CEEC938}"/>
-    <hyperlink ref="A13" r:id="rId10" xr:uid="{604E82EC-6C86-4D9A-B867-F6A20014797C}"/>
+    <hyperlink ref="A12" r:id="rId9" display="KY-016 indicator LED" xr:uid="{6A8AA35F-6C88-4BD6-B333-FC1A2CEEC938}"/>
+    <hyperlink ref="A13" r:id="rId10" display="KY-040 rotary encoders (knobs)" xr:uid="{604E82EC-6C86-4D9A-B867-F6A20014797C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>

</xml_diff>